<commit_message>
added read me file
</commit_message>
<xml_diff>
--- a/output/Optimal_Portfolio_Details.xlsx
+++ b/output/Optimal_Portfolio_Details.xlsx
@@ -502,13 +502,13 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.1875727827201331</v>
+        <v>0.09713344452125153</v>
       </c>
       <c r="D2" t="n">
         <v>0.45504726081112</v>
       </c>
       <c r="E2" t="n">
-        <v>0.3184709763565663</v>
+        <v>0.1649182917956413</v>
       </c>
       <c r="F2" t="n">
         <v>2</v>
@@ -519,16 +519,16 @@
         </is>
       </c>
       <c r="H2" t="n">
-        <v>-0.08602068251076989</v>
+        <v>-0.07287325603580108</v>
       </c>
       <c r="I2" t="n">
         <v>0.08</v>
       </c>
       <c r="J2" t="n">
-        <v>4.540536645768572</v>
+        <v>4.664256048167697</v>
       </c>
       <c r="K2" t="n">
-        <v>1.105419822984372</v>
+        <v>1.255846506602602</v>
       </c>
     </row>
     <row r="3">
@@ -543,13 +543,13 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.1202865336258864</v>
+        <v>0.1357309662849703</v>
       </c>
       <c r="D3" t="n">
         <v>0.7392926196716658</v>
       </c>
       <c r="E3" t="n">
-        <v>0.3815065996495327</v>
+        <v>0.4304909107745751</v>
       </c>
       <c r="F3" t="n">
         <v>2</v>
@@ -560,7 +560,7 @@
         </is>
       </c>
       <c r="H3" t="n">
-        <v>-0.1280393110917985</v>
+        <v>-0.1291799776589777</v>
       </c>
       <c r="I3" t="n">
         <v>0.12</v>
@@ -580,13 +580,13 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.09013830688070659</v>
+        <v>0.03602140854847032</v>
       </c>
       <c r="D4" t="n">
         <v>0.1527853324991495</v>
       </c>
       <c r="E4" t="n">
-        <v>1.789302486095602</v>
+        <v>0.715047776010967</v>
       </c>
       <c r="F4" t="n">
         <v>2</v>
@@ -597,7 +597,7 @@
         </is>
       </c>
       <c r="H4" t="n">
-        <v>0.4944757865019297</v>
+        <v>0.5157574252241206</v>
       </c>
       <c r="I4" t="n">
         <v>0.28</v>
@@ -617,13 +617,13 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.1641518453250353</v>
+        <v>0.1673970425776976</v>
       </c>
       <c r="D5" t="n">
         <v>0.5908724055155681</v>
       </c>
       <c r="E5" t="n">
-        <v>1.02081128054398</v>
+        <v>1.040992192653427</v>
       </c>
       <c r="F5" t="n">
         <v>2</v>
@@ -654,13 +654,13 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.09809633717061136</v>
+        <v>0.1439811213567938</v>
       </c>
       <c r="D6" t="n">
         <v>0.700653114663697</v>
       </c>
       <c r="E6" t="n">
-        <v>0.9292564421997932</v>
+        <v>1.363918250517865</v>
       </c>
       <c r="F6" t="n">
         <v>2</v>
@@ -671,7 +671,7 @@
         </is>
       </c>
       <c r="H6" t="n">
-        <v>-0.1377694141588164</v>
+        <v>-0.1368514987685632</v>
       </c>
       <c r="I6" t="n">
         <v>0.11</v>
@@ -691,13 +691,13 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>-0.1280393110917985</v>
+        <v>-0.1291799776589777</v>
       </c>
       <c r="D7" t="n">
         <v>-0.3737536332074042</v>
       </c>
       <c r="E7" t="n">
-        <v>1.155828241763567</v>
+        <v>1.166125193703865</v>
       </c>
       <c r="F7" t="n">
         <v>2</v>
@@ -728,13 +728,13 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.02382609644082721</v>
+        <v>0.04662796151971213</v>
       </c>
       <c r="D8" t="n">
         <v>0.6550762740412879</v>
       </c>
       <c r="E8" t="n">
-        <v>0.05621132658935624</v>
+        <v>0.1100062521651354</v>
       </c>
       <c r="F8" t="n">
         <v>2</v>
@@ -745,7 +745,7 @@
         </is>
       </c>
       <c r="H8" t="n">
-        <v>0.2899234172528812</v>
+        <v>0.3420446477696094</v>
       </c>
       <c r="I8" t="n">
         <v>0.11</v>
@@ -765,13 +765,13 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.184980570170358</v>
+        <v>0.2280148978263631</v>
       </c>
       <c r="D9" t="n">
         <v>2.364739092345368</v>
       </c>
       <c r="E9" t="n">
-        <v>0.3978290040680159</v>
+        <v>0.4903809066616679</v>
       </c>
       <c r="F9" t="n">
         <v>2</v>
@@ -802,13 +802,13 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>-0.1377694141588164</v>
+        <v>-0.1368514987685632</v>
       </c>
       <c r="D10" t="n">
         <v>-0.2336435907231279</v>
       </c>
       <c r="E10" t="n">
-        <v>1.218552443830876</v>
+        <v>1.210433602295166</v>
       </c>
       <c r="F10" t="n">
         <v>2</v>
@@ -819,7 +819,7 @@
         </is>
       </c>
       <c r="H10" t="n">
-        <v>0.2542901522057419</v>
+        <v>0.2034184511261679</v>
       </c>
       <c r="I10" t="n">
         <v>0.13</v>
@@ -839,13 +839,13 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>-0.08602068251076989</v>
+        <v>-0.07287325603580108</v>
       </c>
       <c r="D11" t="n">
         <v>-0.1533504561112032</v>
       </c>
       <c r="E11" t="n">
-        <v>1.15360469609712</v>
+        <v>0.9772874142478776</v>
       </c>
       <c r="F11" t="n">
         <v>2</v>
@@ -876,13 +876,13 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.1696368836269949</v>
+        <v>0.2063136814846392</v>
       </c>
       <c r="D12" t="n">
         <v>1.156334969843353</v>
       </c>
       <c r="E12" t="n">
-        <v>0.1439873198953499</v>
+        <v>0.1751184849636601</v>
       </c>
       <c r="F12" t="n">
         <v>2</v>
@@ -893,7 +893,7 @@
         </is>
       </c>
       <c r="H12" t="n">
-        <v>-0.1460009164923926</v>
+        <v>-0.09933819709753919</v>
       </c>
       <c r="I12" t="n">
         <v>0.04</v>
@@ -913,13 +913,13 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>-0.1460009164923926</v>
+        <v>-0.09933819709753919</v>
       </c>
       <c r="D13" t="n">
         <v>-0.06308945561220225</v>
       </c>
       <c r="E13" t="n">
-        <v>0.7246084579449813</v>
+        <v>0.4930194929127935</v>
       </c>
       <c r="F13" t="n">
         <v>2</v>

</xml_diff>